<commit_message>
1.0 Ready for fabrication
</commit_message>
<xml_diff>
--- a/v7-soc-8bit/fabrication/BOM.xlsx
+++ b/v7-soc-8bit/fabrication/BOM.xlsx
@@ -19,19 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9" count="9">
-  <si>
-    <t>Designator</t>
-  </si>
-  <si>
-    <t>Footprint</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>JLCPCB Part #</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4" count="4">
   <si>
     <t>R_0603_1608Metric</t>
   </si>
@@ -43,9 +31,6 @@
   </si>
   <si>
     <t>10uF</t>
-  </si>
-  <si>
-    <t>C841192</t>
   </si>
 </sst>
 </file>
@@ -139,12 +124,12 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A1" sqref="A1:D1"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" style="1" width="21.141586538461542" customWidth="1"/>
+    <col min="1" max="1" style="1" width="13.570612980769232" customWidth="1"/>
     <col min="2" max="2" style="1" width="34.56935096153847" customWidth="1"/>
     <col min="3" max="3" style="1" width="25.9984375" customWidth="1"/>
     <col min="4" max="4" style="1" width="14.999098557692308" customWidth="1"/>
@@ -152,17 +137,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16384" customHeight="1" ht="15">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Designator</t>
+        </is>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Footprint</t>
+        </is>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>JLCPCB Part #</t>
+        </is>
       </c>
     </row>
     <row r="2" spans="1:16384">
@@ -194,7 +187,7 @@
         </is>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -203,7 +196,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>C113190</t>
+          <t>C5123581</t>
         </is>
       </c>
     </row>
@@ -236,7 +229,7 @@
         </is>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -256,7 +249,7 @@
         </is>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -320,7 +313,7 @@
         </is>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -329,7 +322,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>C77404</t>
+          <t>C5457064</t>
         </is>
       </c>
     </row>
@@ -340,10 +333,10 @@
         </is>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -358,7 +351,7 @@
         </is>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -378,7 +371,7 @@
         </is>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -398,7 +391,7 @@
         </is>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -418,7 +411,7 @@
         </is>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -491,8 +484,10 @@
           <t>RT9080-33GJ5</t>
         </is>
       </c>
-      <c r="D17" t="s">
-        <v>8</v>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>C841192</t>
+        </is>
       </c>
     </row>
     <row r="18" spans="1:16384">
@@ -502,7 +497,7 @@
         </is>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -544,10 +539,10 @@
         </is>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
S3-SoC sent to production Rel 1.0
</commit_message>
<xml_diff>
--- a/v7-soc-8bit/fabrication/BOM.xlsx
+++ b/v7-soc-8bit/fabrication/BOM.xlsx
@@ -14,12 +14,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
   </definedNames>
   <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
-  <webPublishing allowPng="1" css="0" codePage="1252"/>
+  <webPublishing allowPng="1" css="0" characterSet="UTF-8"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4" count="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6" count="6">
   <si>
     <t>R_0603_1608Metric</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>10uF</t>
+  </si>
+  <si>
+    <t>D_0805</t>
+  </si>
+  <si>
+    <t>LED</t>
   </si>
 </sst>
 </file>
@@ -79,12 +85,12 @@
   </fills>
   <borders count="1">
     <border diagonalUp="0" diagonalDown="0">
-      <left style="none">
+      <start style="none">
         <color rgb="FFC7C7C7"/>
-      </left>
-      <right style="none">
+      </start>
+      <end style="none">
         <color rgb="FFC7C7C7"/>
-      </right>
+      </end>
       <top style="none">
         <color rgb="FFC7C7C7"/>
       </top>
@@ -124,7 +130,7 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -191,12 +197,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>10k</t>
+          <t>10k   BASIC</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>C5123581</t>
+          <t>C25804</t>
         </is>
       </c>
     </row>
@@ -380,7 +386,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>C388041</t>
+          <t>C561172</t>
         </is>
       </c>
     </row>
@@ -395,12 +401,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0Ω</t>
+          <t>0Ω BASIC</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>C3980353</t>
+          <t>C21189</t>
         </is>
       </c>
     </row>
@@ -528,7 +534,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>C201760</t>
+          <t>C3285081</t>
         </is>
       </c>
     </row>
@@ -569,6 +575,64 @@
       <c r="D21" t="inlineStr">
         <is>
           <t>C2827693</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" spans="1:16384">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>D1,D2</t>
+        </is>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>C2297</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" spans="1:16384">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>D3,D4</t>
+        </is>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>C84256</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" spans="1:16384">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>RN1</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>RES_NET_YC124_2X1_YAG</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>4x 0402 Resistor Net.</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>C728735</t>
         </is>
       </c>
     </row>

</xml_diff>